<commit_message>
Purchase Test suites updated
</commit_message>
<xml_diff>
--- a/src/Input_Purchase/input_purc_m.xlsx
+++ b/src/Input_Purchase/input_purc_m.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priti\workspace\JibesFunctionalTest\src\Input_Purchase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priti\workspace\JibeFunctionalTest\src\Input_Purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="217">
   <si>
     <t>Field Labels</t>
   </si>
@@ -379,12 +379,6 @@
     <t>PurchaseConfigsettingsURL</t>
   </si>
   <si>
-    <t>PerchaseConfiSetting</t>
-  </si>
-  <si>
-    <t>2/E</t>
-  </si>
-  <si>
     <t>Select dd_Rank</t>
   </si>
   <si>
@@ -473,6 +467,216 @@
   </si>
   <si>
     <t xml:space="preserve"> Enter Txt_CategoryShortCode</t>
+  </si>
+  <si>
+    <t>TestingLabList</t>
+  </si>
+  <si>
+    <t>http://192.168.1.102/JIBE/Operations/LOAnalysis/LOTestingLabs.aspx</t>
+  </si>
+  <si>
+    <t>AddNewLab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type txt_Lab Name </t>
+  </si>
+  <si>
+    <t>Type txt_Address</t>
+  </si>
+  <si>
+    <t>juinagar, sanpada</t>
+  </si>
+  <si>
+    <t>Type txt_Email</t>
+  </si>
+  <si>
+    <t>rt@gmail.com</t>
+  </si>
+  <si>
+    <t>Type number_Phone</t>
+  </si>
+  <si>
+    <t>Select dd_Country</t>
+  </si>
+  <si>
+    <t>ALAND ISLANDS</t>
+  </si>
+  <si>
+    <t>Verify Newly Added Lab Name</t>
+  </si>
+  <si>
+    <t>Type txt_Code/Desc</t>
+  </si>
+  <si>
+    <t>EditLab</t>
+  </si>
+  <si>
+    <t>Vashi</t>
+  </si>
+  <si>
+    <t>c-sharp pprogg</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>http://192.168.1.102/JIBE/purchase/Location.aspx</t>
+  </si>
+  <si>
+    <t>AddNewLocation</t>
+  </si>
+  <si>
+    <t>Type txt_Short Code</t>
+  </si>
+  <si>
+    <t>Type txt_Short Description</t>
+  </si>
+  <si>
+    <t>Type txt_Long Description</t>
+  </si>
+  <si>
+    <t>COMPANY</t>
+  </si>
+  <si>
+    <t>Type txt_No. of Location</t>
+  </si>
+  <si>
+    <t>Select dd_Vessel Type</t>
+  </si>
+  <si>
+    <t>GAS CARRIER</t>
+  </si>
+  <si>
+    <t>EditLocation</t>
+  </si>
+  <si>
+    <t>Type txt_Short Code/Desc.</t>
+  </si>
+  <si>
+    <t>Highly paid</t>
+  </si>
+  <si>
+    <t>DeleteLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enter Txt_Item Category Name</t>
+  </si>
+  <si>
+    <t>3/E</t>
+  </si>
+  <si>
+    <t>CaptureRank</t>
+  </si>
+  <si>
+    <t>Set Items Min Max Quantity</t>
+  </si>
+  <si>
+    <t>MinMaxQuantityURL</t>
+  </si>
+  <si>
+    <t>http://192.168.1.102/JIBE/purchase/PURC_Items_Quantity_List.aspx</t>
+  </si>
+  <si>
+    <t>CatalogueItem</t>
+  </si>
+  <si>
+    <t>Type txr_Effect Date</t>
+  </si>
+  <si>
+    <t>Type txt_Min Qty</t>
+  </si>
+  <si>
+    <t>Type txt_Max Qty</t>
+  </si>
+  <si>
+    <t>Deck Stores</t>
+  </si>
+  <si>
+    <t>Deck system</t>
+  </si>
+  <si>
+    <t>Deck Subsystem</t>
+  </si>
+  <si>
+    <t>Select dd_Department</t>
+  </si>
+  <si>
+    <t>Select dd_Catalogue</t>
+  </si>
+  <si>
+    <t>Select dd_SubCatalogue</t>
+  </si>
+  <si>
+    <t>LO Testing Lab List</t>
+  </si>
+  <si>
+    <t>01-01-2017</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>http://192.168.1.102/JIBE/Purchase/Purchase_Questionnaire.aspx</t>
+  </si>
+  <si>
+    <t>AddNewQuestion</t>
+  </si>
+  <si>
+    <t>Type txt_Question</t>
+  </si>
+  <si>
+    <t>Select dd_Requisition Type</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Select dd_Grading Type</t>
+  </si>
+  <si>
+    <t>Is this a new grade type?</t>
+  </si>
+  <si>
+    <t>Verify Added Question</t>
+  </si>
+  <si>
+    <t>Type txt_ Search</t>
+  </si>
+  <si>
+    <t>Verify Deleted Question</t>
+  </si>
+  <si>
+    <t>DeleteNewQuestion</t>
+  </si>
+  <si>
+    <t>AddNewGrade</t>
+  </si>
+  <si>
+    <t>Type txt_Grade</t>
+  </si>
+  <si>
+    <t>Grade-A</t>
+  </si>
+  <si>
+    <t>Select dd_Min Point</t>
+  </si>
+  <si>
+    <t>Select dd_Max Point</t>
+  </si>
+  <si>
+    <t>Select dd_No of Options</t>
+  </si>
+  <si>
+    <t>working power?11</t>
+  </si>
+  <si>
+    <t>TeleService</t>
+  </si>
+  <si>
+    <t>77799.00</t>
   </si>
 </sst>
 </file>
@@ -547,7 +751,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,7 +817,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +889,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -717,24 +933,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="3" builtinId="26"/>
@@ -1733,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,11 +1989,11 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
@@ -1770,7 +2001,7 @@
       </c>
       <c r="G3" s="26"/>
       <c r="H3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1790,7 +2021,7 @@
       </c>
       <c r="G5" s="22"/>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1800,7 +2031,7 @@
       <c r="B6" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="26" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1811,19 +2042,19 @@
       <c r="B7" t="s">
         <v>106</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="26" t="s">
         <v>104</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="17" t="s">
         <v>105</v>
       </c>
       <c r="C8" t="s">
@@ -1932,11 +2163,11 @@
       <c r="J16" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
@@ -1955,279 +2186,799 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
-        <v>117</v>
+      <c r="B21" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="27"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="38"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
         <v>122</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C34" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="31"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="35"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" t="s">
         <v>140</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="26" t="s">
         <v>139</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C52" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C53" s="34">
-        <v>22</v>
+        <v>146</v>
+      </c>
+      <c r="C53" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>144</v>
-      </c>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>144</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C56" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B57" t="s">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
         <v>145</v>
       </c>
-      <c r="C57" t="s">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="35"/>
+      <c r="B63" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="35"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>146</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C60" t="s">
-        <v>147</v>
+      <c r="B65" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B68" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="29">
+        <v>1239876789</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="35"/>
+      <c r="B78" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="35"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B83" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C90" s="34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
+      <c r="B93" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C93" s="35"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" t="s">
+        <v>181</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>183</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C98" s="34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>183</v>
+      </c>
+      <c r="B99" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>183</v>
+      </c>
+      <c r="B100" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>183</v>
+      </c>
+      <c r="B101" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>183</v>
+      </c>
+      <c r="B102" t="s">
+        <v>191</v>
+      </c>
+      <c r="C102" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>183</v>
+      </c>
+      <c r="B103" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="35"/>
+      <c r="B106" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C106" s="35"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="49" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="41"/>
+      <c r="B108" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C108" s="41"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="C109" s="47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="C110" s="48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B111" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="C111" s="48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="44"/>
+      <c r="B112" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="41"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B113" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C113" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B114" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="C114" s="41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="41"/>
+      <c r="B115" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="C115" s="41"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C116" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="C117" s="41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="41"/>
+      <c r="B118" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C118" s="41"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B119" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="C119" s="48" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B120" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="C120" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B121" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="C121" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B122" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="C122" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C159" t="s">
+        <v>171</v>
+      </c>
+      <c r="D159" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C20" r:id="rId2"/>
+    <hyperlink ref="C69" r:id="rId3"/>
+    <hyperlink ref="C79" r:id="rId4"/>
+    <hyperlink ref="C107" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>